<commit_message>
Redid some files and added more references again.
</commit_message>
<xml_diff>
--- a/cold_genes_combined_with_gene_interval_update_01052017.xlsx
+++ b/cold_genes_combined_with_gene_interval_update_01052017.xlsx
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$157</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="439">
   <si>
     <t>Gene_Chr</t>
   </si>
@@ -1287,55 +1288,67 @@
     <t>reference</t>
   </si>
   <si>
-    <t>PMC146917</t>
-  </si>
-  <si>
-    <t>Gapped BLAST and PSI-BLAST: a new generation of protein database search programs.</t>
-  </si>
-  <si>
-    <t>Subdivision and haplotype structure in natural populations of Arabidopsis lyrata.</t>
-  </si>
-  <si>
-    <t>Wiley</t>
-  </si>
-  <si>
-    <t>PMC2528102</t>
-  </si>
-  <si>
-    <t>Global analysis of Arabidopsis gene expression uncovers a complex array of changes impacting pathogen response and cell cycle during geminivirus infection.</t>
-  </si>
-  <si>
-    <t>PMC1276035</t>
-  </si>
-  <si>
-    <t>The Arabidopsis cold-responsive transcriptome and its regulation by ICE1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMC166537 </t>
-  </si>
-  <si>
     <t>Inositol phospholipid metabolism in Arabidopsis. Characterized and putative isoforms of inositol phospholipid kinase and phosphoinositide-specific phospholipase C.</t>
   </si>
   <si>
-    <t>Characterization of the Sucrose Phosphate Phosphatase (SPP) Isoforms from Arabidopsis thaliana and Role of the S6PPc Domain in Dimerization</t>
-  </si>
-  <si>
-    <t>Characterization of two distinct subfamilies of SUN-domain proteins in Arabidopsis and their interactions with the novel KASH-domain protein AtTIK</t>
-  </si>
-  <si>
-    <t>Biochemical and structural study of Arabidopsis hexokinase 1</t>
-  </si>
-  <si>
-    <t>Transgenic expression of MYB15 confers enhanced sensitivity to abscisic acid and improved drought tolerance in Arabidopsis thaliana</t>
-  </si>
-  <si>
-    <t>Cross genome comparisons of serine proteases in Arabidopsis and rice.</t>
+    <t>12-oxophytodienoate reductase 3 (OPR3) is the isoenzyme involved in jasmonate biosynthesis.</t>
+  </si>
+  <si>
+    <t>12-Oxo-Phytodienoic Acid Triggers Expression of a Distinct Set of Genes and Plays a Role in Wound-Induced Gene Expression in Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Arabidopsis AtDGK7, the smallest member of plant diacylglycerol kinases, displays unique biochemical features and saturates at low substrate concentration-the DGK inhibitor R59022 differentially affects AtDGK2 and AtDGK7 activity in vitro, and alters plant growth and development.</t>
+  </si>
+  <si>
+    <t>Molecular cloning of a cDNA encoding diacylglycerol kinase (DGK) in Arabidopsis thaliana.</t>
+  </si>
+  <si>
+    <t>Sucrose-phosphatase gene families in plants.</t>
+  </si>
+  <si>
+    <t>Expression of Arabidopsis Hexokinase in Citrus Guard Cells Controls Stomatal Aperture and Reduces Transpiration</t>
+  </si>
+  <si>
+    <t>A R2R3-type myb transcription factor is involved in the cold-regulation of CBF genes and in acquired freezing tolerance.</t>
   </si>
   <si>
     <t>Phospholipid-derived signaling mediated by phospholipase A in plants.</t>
   </si>
   <si>
+    <t>Transgressive segregation reveals two Arabidopsis TIR-NB-LRR resistance genes effective against Leptosphaeria maculans, causal agent of blackleg disease.</t>
+  </si>
+  <si>
     <t>Identification of phosphomethylethanolamine N-methyltransferase from Arabidopsis and its role in choline and phospholipid metabolism</t>
+  </si>
+  <si>
+    <t>PHOSPHATIDIC ACID PHOSPHOHYDROLASE1 and 2 Regulate Phospholipid Synthesis at the Endoplasmic Reticulum in Arabidopsis</t>
+  </si>
+  <si>
+    <t>PMC152217</t>
+  </si>
+  <si>
+    <t>The Arabidopsis phospholipase D family. Characterization of a calcium-independent and phosphatidylcholine-selective PLD zeta 1 with distinct regulatory domains.</t>
+  </si>
+  <si>
+    <t>The Choline/Ethanolamine Kinase Family in Arabidopsis: Essential Role of CEK4 in Phospholipid Biosynthesis and Embryo Development</t>
+  </si>
+  <si>
+    <t>Handling calcium signaling: Arabidopsis CaMs and CMLs.</t>
+  </si>
+  <si>
+    <t>Calmodulin isoforms in Arabidopsis encoded by multiple divergent mRNAs.</t>
+  </si>
+  <si>
+    <t>Functional genomic analysis of Arabidopsis thaliana glycoside hydrolase family 1.</t>
+  </si>
+  <si>
+    <t>A bifunctional TPS-TPP enzyme from yeast confers tolerance to multiple and extreme abiotic-stress conditions in transgenic Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Overexpression of the trehalose-6-phosphate phosphatase gene OsTPP1 confers stress tolerance in rice and results in the activation of stress responsive genes.</t>
+  </si>
+  <si>
+    <t>OST1 Kinase Modulates Freezing Tolerance by Enhancing ICE1 Stability in Arabidopsis</t>
   </si>
 </sst>
 </file>
@@ -1559,7 +1572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1602,12 +1615,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1770,28 +1809,53 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2100,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.4" x14ac:dyDescent="0.5"/>
@@ -2170,7 +2234,7 @@
       <c r="O1" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="62" t="s">
         <v>416</v>
       </c>
       <c r="Q1" s="11" t="s">
@@ -2236,13 +2300,13 @@
       <c r="N2" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="O2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="55" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q2" s="56" t="s">
+      <c r="O2" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="55">
+        <v>10872231</v>
+      </c>
+      <c r="Q2" s="70" t="s">
         <v>419</v>
       </c>
     </row>
@@ -2289,14 +2353,14 @@
       <c r="N3" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="O3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="55" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q3" s="56" t="s">
-        <v>419</v>
+      <c r="O3" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="55">
+        <v>16258017</v>
+      </c>
+      <c r="Q3" s="70" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:35" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
@@ -2340,15 +2404,11 @@
       <c r="N4" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="O4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q4" s="56" t="s">
-        <v>420</v>
-      </c>
+      <c r="O4" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="61"/>
     </row>
     <row r="5" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="17" t="s">
@@ -2391,12 +2451,8 @@
       <c r="O5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q5" s="56" t="s">
-        <v>420</v>
-      </c>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="61"/>
     </row>
     <row r="6" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="17" t="s">
@@ -2442,12 +2498,8 @@
       <c r="O6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="59" t="s">
-        <v>422</v>
-      </c>
-      <c r="Q6" s="58" t="s">
-        <v>423</v>
-      </c>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="56"/>
       <c r="R6" s="19"/>
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
@@ -2507,11 +2559,11 @@
       <c r="M7" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="P7" s="59" t="s">
-        <v>424</v>
-      </c>
-      <c r="Q7" s="60" t="s">
-        <v>425</v>
+      <c r="P7" s="55">
+        <v>16081412</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:35" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
@@ -2558,11 +2610,11 @@
       <c r="O8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="59" t="s">
-        <v>424</v>
-      </c>
-      <c r="Q8" s="60" t="s">
-        <v>425</v>
+      <c r="P8" s="58">
+        <v>8605313</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>422</v>
       </c>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
@@ -2624,11 +2676,11 @@
       <c r="O9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="59" t="s">
-        <v>426</v>
-      </c>
-      <c r="Q9" s="58" t="s">
-        <v>427</v>
+      <c r="P9" s="57">
+        <v>12226484</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="10" spans="1:35" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
@@ -2675,11 +2727,11 @@
       <c r="O10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="61">
-        <v>27855180</v>
-      </c>
-      <c r="Q10" s="62" t="s">
-        <v>428</v>
+      <c r="P10" s="55">
+        <v>12559580</v>
+      </c>
+      <c r="Q10" s="47" t="s">
+        <v>423</v>
       </c>
       <c r="R10" s="47"/>
       <c r="S10" s="47"/>
@@ -2743,12 +2795,8 @@
       <c r="O11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P11" s="55">
-        <v>25217773</v>
-      </c>
-      <c r="Q11" s="58" t="s">
-        <v>429</v>
-      </c>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="56"/>
     </row>
     <row r="12" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A12" s="17" t="s">
@@ -2791,11 +2839,11 @@
       <c r="O12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="55">
-        <v>25664748</v>
-      </c>
-      <c r="Q12" s="58" t="s">
-        <v>430</v>
+      <c r="P12" s="57">
+        <v>26734024</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
@@ -2845,10 +2893,10 @@
         <v>22</v>
       </c>
       <c r="P13" s="55">
-        <v>19161942</v>
-      </c>
-      <c r="Q13" s="58" t="s">
-        <v>431</v>
+        <v>17015446</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="14" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
@@ -2895,12 +2943,8 @@
       <c r="O14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P14" s="55">
-        <v>16895613</v>
-      </c>
-      <c r="Q14" s="58" t="s">
-        <v>432</v>
-      </c>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="56"/>
       <c r="R14" s="19"/>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
@@ -2966,8 +3010,8 @@
       <c r="P15" s="55">
         <v>15130548</v>
       </c>
-      <c r="Q15" s="60" t="s">
-        <v>433</v>
+      <c r="Q15" s="21" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="16" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
@@ -3013,6 +3057,7 @@
       <c r="O16" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P16" s="64"/>
     </row>
     <row r="17" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A17" s="19" t="s">
@@ -3057,6 +3102,7 @@
       <c r="O17" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P17" s="64"/>
     </row>
     <row r="18" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="17" t="s">
@@ -3102,8 +3148,12 @@
       <c r="O18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
+      <c r="P18" s="55">
+        <v>16623885</v>
+      </c>
+      <c r="Q18" s="19" t="s">
+        <v>427</v>
+      </c>
       <c r="R18" s="19"/>
       <c r="S18" s="19"/>
       <c r="T18" s="19"/>
@@ -3169,11 +3219,11 @@
       <c r="O19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="63">
+      <c r="P19" s="55">
         <v>20650897</v>
       </c>
-      <c r="Q19" s="60" t="s">
-        <v>434</v>
+      <c r="Q19" s="21" t="s">
+        <v>428</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -3240,11 +3290,11 @@
       <c r="O20" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P20" s="63">
-        <v>20650897</v>
-      </c>
-      <c r="Q20" s="60" t="s">
-        <v>434</v>
+      <c r="P20" s="55">
+        <v>20699392</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>429</v>
       </c>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
@@ -3308,6 +3358,12 @@
       <c r="O21" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P21" s="55" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q21" s="19" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="22" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A22" s="29" t="s">
@@ -3353,8 +3409,12 @@
       <c r="O22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
+      <c r="P22" s="55">
+        <v>25966764</v>
+      </c>
+      <c r="Q22" s="19" t="s">
+        <v>432</v>
+      </c>
       <c r="R22" s="19"/>
       <c r="S22" s="19"/>
       <c r="T22" s="19"/>
@@ -3417,6 +3477,7 @@
       <c r="O23" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P23" s="64"/>
     </row>
     <row r="24" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="23" t="s">
@@ -3464,8 +3525,12 @@
       <c r="O24" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
+      <c r="P24" s="71">
+        <v>16023399</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>433</v>
+      </c>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -3529,8 +3594,12 @@
       <c r="O25" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="P25" s="55">
+        <v>8507825</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -3596,6 +3665,12 @@
       <c r="O26" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P26" s="72">
+        <v>15604686</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="27" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="s">
@@ -3640,6 +3715,12 @@
       <c r="O27" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P27" s="55">
+        <v>17628825</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="28" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
@@ -3685,8 +3766,12 @@
       <c r="O28" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+      <c r="P28" s="57">
+        <v>18365248</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -3706,7 +3791,7 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="19" t="s">
         <v>306</v>
       </c>
@@ -3748,6 +3833,12 @@
       </c>
       <c r="O29" s="21" t="s">
         <v>22</v>
+      </c>
+      <c r="P29" s="55">
+        <v>25669882</v>
+      </c>
+      <c r="Q29" s="19" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.5">
@@ -3796,7 +3887,7 @@
       <c r="O30" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P30" s="4"/>
+      <c r="P30" s="66"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
@@ -3861,7 +3952,7 @@
       <c r="O31" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P31" s="19"/>
+      <c r="P31" s="64"/>
       <c r="Q31" s="19"/>
       <c r="R31" s="19"/>
       <c r="S31" s="19"/>
@@ -3926,7 +4017,7 @@
       <c r="O32" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P32" s="19"/>
+      <c r="P32" s="64"/>
       <c r="Q32" s="19"/>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
@@ -3991,7 +4082,7 @@
       <c r="O33" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P33" s="19"/>
+      <c r="P33" s="64"/>
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
       <c r="S33" s="19"/>
@@ -4056,7 +4147,7 @@
       <c r="O34" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P34" s="4"/>
+      <c r="P34" s="66"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
@@ -4123,6 +4214,7 @@
       <c r="O35" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P35" s="65"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A36" s="21" t="s">
@@ -4167,6 +4259,7 @@
       <c r="O36" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P36" s="53"/>
     </row>
     <row r="37" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A37" s="28" t="s">
@@ -4214,7 +4307,7 @@
       <c r="O37" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P37" s="21"/>
+      <c r="P37" s="53"/>
       <c r="Q37" s="21"/>
       <c r="R37" s="21"/>
       <c r="S37" s="21"/>
@@ -4278,6 +4371,7 @@
       <c r="O38" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P38" s="64"/>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A39" s="19" t="s">
@@ -4323,7 +4417,7 @@
       <c r="O39" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P39" s="19"/>
+      <c r="P39" s="64"/>
       <c r="Q39" s="19"/>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
@@ -4388,7 +4482,7 @@
       <c r="O40" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="19"/>
+      <c r="P40" s="64"/>
       <c r="Q40" s="19"/>
       <c r="R40" s="19"/>
       <c r="S40" s="19"/>
@@ -4453,7 +4547,7 @@
       <c r="O41" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P41" s="19"/>
+      <c r="P41" s="64"/>
       <c r="Q41" s="19"/>
       <c r="R41" s="19"/>
       <c r="S41" s="19"/>
@@ -4520,7 +4614,7 @@
       <c r="O42" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P42" s="4"/>
+      <c r="P42" s="66"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
@@ -4581,7 +4675,7 @@
       <c r="O43" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P43" s="19"/>
+      <c r="P43" s="64"/>
       <c r="Q43" s="19"/>
       <c r="R43" s="19"/>
       <c r="S43" s="19"/>
@@ -4642,7 +4736,7 @@
       <c r="O44" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P44" s="21"/>
+      <c r="P44" s="53"/>
       <c r="Q44" s="21"/>
       <c r="R44" s="21"/>
       <c r="S44" s="21"/>
@@ -4706,6 +4800,7 @@
       <c r="O45" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P45" s="64"/>
     </row>
     <row r="46" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A46" s="19" t="s">
@@ -4750,6 +4845,7 @@
       <c r="O46" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P46" s="64"/>
     </row>
     <row r="47" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A47" s="19" t="s">
@@ -4794,6 +4890,7 @@
       <c r="O47" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P47" s="64"/>
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A48" s="19" t="s">
@@ -4839,7 +4936,7 @@
       <c r="O48" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P48" s="19"/>
+      <c r="P48" s="64"/>
       <c r="Q48" s="19"/>
       <c r="R48" s="19"/>
       <c r="S48" s="19"/>
@@ -4904,7 +5001,7 @@
       <c r="O49" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P49" s="19"/>
+      <c r="P49" s="64"/>
       <c r="Q49" s="19"/>
       <c r="R49" s="19"/>
       <c r="S49" s="19"/>
@@ -4969,7 +5066,7 @@
       <c r="O50" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P50" s="19"/>
+      <c r="P50" s="64"/>
       <c r="Q50" s="19"/>
       <c r="R50" s="19"/>
       <c r="S50" s="19"/>
@@ -5030,7 +5127,7 @@
       <c r="O51" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P51" s="19"/>
+      <c r="P51" s="64"/>
       <c r="Q51" s="19"/>
       <c r="R51" s="19"/>
       <c r="S51" s="19"/>
@@ -5095,7 +5192,7 @@
       <c r="O52" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P52" s="19"/>
+      <c r="P52" s="64"/>
       <c r="Q52" s="19"/>
       <c r="R52" s="19"/>
       <c r="S52" s="19"/>
@@ -5162,7 +5259,7 @@
       <c r="O53" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P53" s="4"/>
+      <c r="P53" s="66"/>
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
@@ -5229,7 +5326,7 @@
       <c r="O54" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="P54" s="36"/>
+      <c r="P54" s="67"/>
       <c r="Q54" s="36"/>
       <c r="R54" s="36"/>
       <c r="S54" s="36"/>
@@ -5294,7 +5391,7 @@
       <c r="O55" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P55" s="21"/>
+      <c r="P55" s="53"/>
       <c r="Q55" s="21"/>
       <c r="R55" s="21"/>
       <c r="S55" s="21"/>
@@ -5361,7 +5458,7 @@
       <c r="O56" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P56" s="4"/>
+      <c r="P56" s="66"/>
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
       <c r="S56" s="4"/>
@@ -5428,7 +5525,7 @@
       <c r="O57" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P57" s="3"/>
+      <c r="P57" s="65"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
@@ -5489,7 +5586,7 @@
       <c r="O58" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P58" s="19"/>
+      <c r="P58" s="64"/>
       <c r="Q58" s="19"/>
       <c r="R58" s="19"/>
       <c r="S58" s="19"/>
@@ -5551,6 +5648,7 @@
       <c r="O59" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P59" s="53"/>
     </row>
     <row r="60" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A60" s="19" t="s">
@@ -5595,6 +5693,7 @@
       <c r="O60" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P60" s="64"/>
     </row>
     <row r="61" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A61" s="19" t="s">
@@ -5639,6 +5738,7 @@
       <c r="O61" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P61" s="64"/>
     </row>
     <row r="62" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A62" s="4" t="s">
@@ -5686,7 +5786,7 @@
       <c r="O62" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P62" s="4"/>
+      <c r="P62" s="66"/>
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
       <c r="S62" s="4"/>
@@ -5753,7 +5853,7 @@
       <c r="O63" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P63" s="4"/>
+      <c r="P63" s="66"/>
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
       <c r="S63" s="4"/>
@@ -5817,6 +5917,7 @@
       <c r="O64" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P64" s="64"/>
     </row>
     <row r="65" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A65" s="19" t="s">
@@ -5861,6 +5962,7 @@
       <c r="O65" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P65" s="64"/>
     </row>
     <row r="66" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A66" s="4" t="s">
@@ -5908,6 +6010,7 @@
       <c r="O66" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P66" s="66"/>
     </row>
     <row r="67" spans="1:35" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="s">
@@ -5953,7 +6056,7 @@
       <c r="O67" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P67" s="3"/>
+      <c r="P67" s="65"/>
       <c r="Q67" s="3"/>
       <c r="R67" s="3"/>
       <c r="S67" s="3"/>
@@ -6018,7 +6121,7 @@
       <c r="O68" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P68" s="3"/>
+      <c r="P68" s="65"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
       <c r="S68" s="3"/>
@@ -6083,7 +6186,7 @@
       <c r="O69" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P69" s="4"/>
+      <c r="P69" s="66"/>
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
       <c r="S69" s="4"/>
@@ -6148,7 +6251,7 @@
       <c r="O70" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P70" s="19"/>
+      <c r="P70" s="64"/>
       <c r="Q70" s="19"/>
       <c r="R70" s="19"/>
       <c r="S70" s="19"/>
@@ -6212,6 +6315,7 @@
       <c r="O71" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P71" s="64"/>
     </row>
     <row r="72" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A72" s="19" t="s">
@@ -6256,6 +6360,7 @@
       <c r="O72" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P72" s="64"/>
     </row>
     <row r="73" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A73" s="19" t="s">
@@ -6300,6 +6405,7 @@
       <c r="O73" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P73" s="64"/>
     </row>
     <row r="74" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A74" s="19" t="s">
@@ -6344,6 +6450,7 @@
       <c r="O74" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P74" s="64"/>
     </row>
     <row r="75" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="s">
@@ -6391,7 +6498,7 @@
       <c r="O75" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P75" s="3"/>
+      <c r="P75" s="65"/>
       <c r="Q75" s="3"/>
       <c r="R75" s="3"/>
       <c r="S75" s="3"/>
@@ -6458,7 +6565,7 @@
       <c r="O76" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P76" s="3"/>
+      <c r="P76" s="65"/>
       <c r="Q76" s="3"/>
       <c r="R76" s="3"/>
       <c r="S76" s="3"/>
@@ -6523,7 +6630,7 @@
       <c r="O77" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P77" s="19"/>
+      <c r="P77" s="64"/>
       <c r="Q77" s="19"/>
       <c r="R77" s="19"/>
       <c r="S77" s="19"/>
@@ -6588,7 +6695,7 @@
       <c r="O78" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P78" s="19"/>
+      <c r="P78" s="64"/>
       <c r="Q78" s="19"/>
       <c r="R78" s="19"/>
       <c r="S78" s="19"/>
@@ -6652,6 +6759,7 @@
       <c r="O79" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P79" s="64"/>
     </row>
     <row r="80" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A80" s="19" t="s">
@@ -6696,6 +6804,7 @@
       <c r="O80" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P80" s="64"/>
     </row>
     <row r="81" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A81" s="3" t="s">
@@ -6743,7 +6852,7 @@
       <c r="O81" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P81" s="21"/>
+      <c r="P81" s="53"/>
       <c r="Q81" s="21"/>
       <c r="R81" s="21"/>
       <c r="S81" s="21"/>
@@ -6810,7 +6919,7 @@
       <c r="O82" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P82" s="3"/>
+      <c r="P82" s="65"/>
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
       <c r="S82" s="3"/>
@@ -6877,6 +6986,7 @@
       <c r="O83" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P83" s="66"/>
     </row>
     <row r="84" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="s">
@@ -6924,7 +7034,7 @@
       <c r="O84" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P84" s="3"/>
+      <c r="P84" s="65"/>
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
       <c r="S84" s="3"/>
@@ -6989,7 +7099,7 @@
       <c r="O85" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P85" s="21"/>
+      <c r="P85" s="53"/>
       <c r="Q85" s="21"/>
       <c r="R85" s="21"/>
       <c r="S85" s="21"/>
@@ -7053,6 +7163,7 @@
       <c r="O86" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P86" s="53"/>
     </row>
     <row r="87" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A87" s="23" t="s">
@@ -7100,7 +7211,7 @@
       <c r="O87" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P87" s="3"/>
+      <c r="P87" s="65"/>
       <c r="Q87" s="3"/>
       <c r="R87" s="3"/>
       <c r="S87" s="3"/>
@@ -7165,7 +7276,7 @@
       <c r="O88" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P88" s="21"/>
+      <c r="P88" s="53"/>
       <c r="Q88" s="21"/>
       <c r="R88" s="21"/>
       <c r="S88" s="21"/>
@@ -7230,7 +7341,7 @@
       <c r="O89" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P89" s="4"/>
+      <c r="P89" s="66"/>
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
       <c r="S89" s="4"/>
@@ -7295,7 +7406,7 @@
       <c r="O90" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P90" s="19"/>
+      <c r="P90" s="64"/>
       <c r="Q90" s="19"/>
       <c r="R90" s="19"/>
       <c r="S90" s="19"/>
@@ -7359,6 +7470,7 @@
       <c r="O91" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P91" s="64"/>
     </row>
     <row r="92" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A92" s="19" t="s">
@@ -7404,7 +7516,7 @@
       <c r="O92" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P92" s="19"/>
+      <c r="P92" s="64"/>
       <c r="Q92" s="19"/>
       <c r="R92" s="19"/>
       <c r="S92" s="19"/>
@@ -7471,7 +7583,7 @@
       <c r="O93" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P93" s="4"/>
+      <c r="P93" s="66"/>
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
       <c r="S93" s="4"/>
@@ -7535,6 +7647,7 @@
       <c r="O94" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P94" s="64"/>
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A95" s="19" t="s">
@@ -7580,7 +7693,7 @@
       <c r="O95" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P95" s="19"/>
+      <c r="P95" s="64"/>
       <c r="Q95" s="19"/>
       <c r="R95" s="19"/>
       <c r="S95" s="19"/>
@@ -7645,7 +7758,7 @@
       <c r="O96" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P96" s="19"/>
+      <c r="P96" s="64"/>
       <c r="Q96" s="19"/>
       <c r="R96" s="19"/>
       <c r="S96" s="19"/>
@@ -7710,7 +7823,7 @@
       <c r="O97" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P97" s="21"/>
+      <c r="P97" s="53"/>
       <c r="Q97" s="21"/>
       <c r="R97" s="21"/>
       <c r="S97" s="21"/>
@@ -7774,6 +7887,7 @@
       <c r="O98" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P98" s="53"/>
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A99" s="21" t="s">
@@ -7818,6 +7932,7 @@
       <c r="O99" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P99" s="53"/>
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A100" s="21" t="s">
@@ -7862,6 +7977,7 @@
       <c r="O100" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P100" s="53"/>
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A101" s="21" t="s">
@@ -7906,6 +8022,7 @@
       <c r="O101" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P101" s="53"/>
     </row>
     <row r="102" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A102" s="21" t="s">
@@ -7950,6 +8067,7 @@
       <c r="O102" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P102" s="53"/>
     </row>
     <row r="103" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A103" s="19" t="s">
@@ -7995,7 +8113,7 @@
       <c r="O103" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P103" s="19"/>
+      <c r="P103" s="64"/>
       <c r="Q103" s="19"/>
       <c r="R103" s="19"/>
       <c r="S103" s="19"/>
@@ -8060,7 +8178,7 @@
       <c r="O104" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P104" s="21"/>
+      <c r="P104" s="53"/>
       <c r="Q104" s="21"/>
       <c r="R104" s="21"/>
       <c r="S104" s="21"/>
@@ -8125,7 +8243,7 @@
       <c r="O105" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P105" s="21"/>
+      <c r="P105" s="53"/>
       <c r="Q105" s="21"/>
       <c r="R105" s="21"/>
       <c r="S105" s="21"/>
@@ -8190,7 +8308,7 @@
       <c r="O106" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P106" s="21"/>
+      <c r="P106" s="53"/>
       <c r="Q106" s="21"/>
       <c r="R106" s="21"/>
       <c r="S106" s="21"/>
@@ -8255,7 +8373,7 @@
       <c r="O107" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P107" s="21"/>
+      <c r="P107" s="53"/>
       <c r="Q107" s="21"/>
       <c r="R107" s="21"/>
       <c r="S107" s="21"/>
@@ -8320,7 +8438,7 @@
       <c r="O108" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P108" s="21"/>
+      <c r="P108" s="53"/>
       <c r="Q108" s="21"/>
       <c r="R108" s="21"/>
       <c r="S108" s="21"/>
@@ -8385,7 +8503,7 @@
       <c r="O109" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P109" s="21"/>
+      <c r="P109" s="53"/>
       <c r="Q109" s="21"/>
       <c r="R109" s="21"/>
       <c r="S109" s="21"/>
@@ -8450,7 +8568,7 @@
       <c r="O110" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P110" s="21"/>
+      <c r="P110" s="53"/>
       <c r="Q110" s="21"/>
       <c r="R110" s="21"/>
       <c r="S110" s="21"/>
@@ -8515,7 +8633,7 @@
       <c r="O111" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P111" s="21"/>
+      <c r="P111" s="53"/>
       <c r="Q111" s="21"/>
       <c r="R111" s="21"/>
       <c r="S111" s="21"/>
@@ -8582,6 +8700,7 @@
       <c r="O112" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P112" s="64"/>
     </row>
     <row r="113" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A113" s="19" t="s">
@@ -8627,7 +8746,7 @@
       <c r="O113" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P113" s="19"/>
+      <c r="P113" s="64"/>
       <c r="Q113" s="19"/>
       <c r="R113" s="19"/>
       <c r="S113" s="19"/>
@@ -8694,7 +8813,7 @@
       <c r="O114" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P114" s="4"/>
+      <c r="P114" s="66"/>
       <c r="Q114" s="4"/>
       <c r="R114" s="4"/>
       <c r="S114" s="4"/>
@@ -8758,6 +8877,7 @@
       <c r="O115" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P115" s="64"/>
     </row>
     <row r="116" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A116" s="19" t="s">
@@ -8803,7 +8923,7 @@
       <c r="O116" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P116" s="19"/>
+      <c r="P116" s="64"/>
       <c r="Q116" s="19"/>
       <c r="R116" s="19"/>
       <c r="S116" s="19"/>
@@ -8868,7 +8988,7 @@
       <c r="O117" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P117" s="19"/>
+      <c r="P117" s="64"/>
       <c r="Q117" s="19"/>
       <c r="R117" s="19"/>
       <c r="S117" s="19"/>
@@ -8933,7 +9053,7 @@
       <c r="O118" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P118" s="19"/>
+      <c r="P118" s="64"/>
       <c r="Q118" s="19"/>
       <c r="R118" s="19"/>
       <c r="S118" s="19"/>
@@ -9000,7 +9120,7 @@
       <c r="O119" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P119" s="3"/>
+      <c r="P119" s="65"/>
       <c r="Q119" s="3"/>
       <c r="R119" s="3"/>
       <c r="S119" s="3"/>
@@ -9064,6 +9184,7 @@
       <c r="O120" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P120" s="64"/>
     </row>
     <row r="121" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A121" s="19" t="s">
@@ -9108,6 +9229,7 @@
       <c r="O121" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P121" s="64"/>
     </row>
     <row r="122" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A122" s="17" t="s">
@@ -9155,6 +9277,7 @@
       <c r="O122" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P122" s="64"/>
     </row>
     <row r="123" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A123" s="19" t="s">
@@ -9199,6 +9322,7 @@
       <c r="O123" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P123" s="64"/>
     </row>
     <row r="124" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A124" s="19" t="s">
@@ -9244,7 +9368,7 @@
       <c r="O124" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P124" s="19"/>
+      <c r="P124" s="64"/>
       <c r="Q124" s="19"/>
       <c r="R124" s="19"/>
       <c r="S124" s="19"/>
@@ -9309,7 +9433,7 @@
       <c r="O125" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P125" s="19"/>
+      <c r="P125" s="64"/>
       <c r="Q125" s="19"/>
       <c r="R125" s="19"/>
       <c r="S125" s="19"/>
@@ -9374,7 +9498,7 @@
       <c r="O126" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P126" s="19"/>
+      <c r="P126" s="64"/>
       <c r="Q126" s="19"/>
       <c r="R126" s="19"/>
       <c r="S126" s="19"/>
@@ -9438,6 +9562,7 @@
       <c r="O127" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P127" s="64"/>
     </row>
     <row r="128" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A128" s="17" t="s">
@@ -9483,7 +9608,7 @@
       <c r="O128" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P128" s="21"/>
+      <c r="P128" s="53"/>
       <c r="Q128" s="21"/>
       <c r="R128" s="21"/>
       <c r="S128" s="21"/>
@@ -9550,7 +9675,7 @@
       <c r="O129" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="P129" s="6"/>
+      <c r="P129" s="68"/>
       <c r="Q129" s="6"/>
       <c r="R129" s="6"/>
       <c r="S129" s="6"/>
@@ -9615,7 +9740,7 @@
       <c r="O130" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="P130" s="36"/>
+      <c r="P130" s="67"/>
       <c r="Q130" s="36"/>
       <c r="R130" s="36"/>
       <c r="S130" s="36"/>
@@ -9680,7 +9805,7 @@
       <c r="O131" s="44" t="s">
         <v>411</v>
       </c>
-      <c r="P131" s="44"/>
+      <c r="P131" s="69"/>
       <c r="Q131" s="44"/>
       <c r="R131" s="44"/>
       <c r="S131" s="44"/>
@@ -9744,6 +9869,7 @@
       <c r="O132" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P132" s="64"/>
     </row>
     <row r="133" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A133" s="3" t="s">
@@ -9791,7 +9917,7 @@
       <c r="O133" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P133" s="3"/>
+      <c r="P133" s="65"/>
       <c r="Q133" s="3"/>
       <c r="R133" s="3"/>
       <c r="S133" s="3"/>
@@ -9858,6 +9984,7 @@
       <c r="O134" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P134" s="65"/>
     </row>
     <row r="135" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A135" s="21" t="s">
@@ -9903,7 +10030,7 @@
       <c r="O135" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P135" s="21"/>
+      <c r="P135" s="53"/>
       <c r="Q135" s="21"/>
       <c r="R135" s="21"/>
       <c r="S135" s="21"/>
@@ -9966,7 +10093,7 @@
       <c r="O136" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P136" s="21"/>
+      <c r="P136" s="53"/>
       <c r="Q136" s="21"/>
       <c r="R136" s="21"/>
       <c r="S136" s="21"/>
@@ -10024,6 +10151,7 @@
       <c r="O137" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P137" s="64"/>
     </row>
     <row r="138" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A138" s="19" t="s">
@@ -10068,6 +10196,7 @@
       <c r="O138" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P138" s="64"/>
     </row>
     <row r="139" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A139" s="3" t="s">
@@ -10115,7 +10244,7 @@
       <c r="O139" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P139" s="3"/>
+      <c r="P139" s="65"/>
       <c r="Q139" s="3"/>
       <c r="R139" s="3"/>
       <c r="S139" s="3"/>
@@ -10179,6 +10308,7 @@
       <c r="O140" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P140" s="64"/>
     </row>
     <row r="141" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A141" s="19" t="s">
@@ -10223,6 +10353,7 @@
       <c r="O141" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P141" s="64"/>
     </row>
     <row r="142" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A142" s="21"/>
@@ -10264,7 +10395,7 @@
       <c r="O142" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P142" s="21"/>
+      <c r="P142" s="53"/>
       <c r="Q142" s="21"/>
       <c r="R142" s="21"/>
       <c r="S142" s="21"/>
@@ -10322,6 +10453,7 @@
       <c r="O143" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P143" s="64"/>
     </row>
     <row r="144" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C144" s="19" t="s">
@@ -10360,6 +10492,7 @@
       <c r="O144" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P144" s="64"/>
     </row>
     <row r="145" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A145" s="17" t="s">
@@ -10407,6 +10540,7 @@
       <c r="O145" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P145" s="64"/>
     </row>
     <row r="146" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A146" s="17" t="s">
@@ -10451,6 +10585,7 @@
       <c r="O146" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P146" s="64"/>
     </row>
     <row r="147" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A147" s="19" t="s">
@@ -10495,6 +10630,7 @@
       <c r="O147" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P147" s="64"/>
     </row>
     <row r="148" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A148" s="17" t="s">
@@ -10538,7 +10674,7 @@
       <c r="O148" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P148" s="21"/>
+      <c r="P148" s="53"/>
       <c r="Q148" s="21"/>
       <c r="R148" s="21"/>
       <c r="S148" s="21"/>
@@ -10605,7 +10741,7 @@
       <c r="O149" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P149" s="3"/>
+      <c r="P149" s="65"/>
       <c r="Q149" s="3"/>
       <c r="R149" s="3"/>
       <c r="S149" s="3"/>
@@ -10672,7 +10808,7 @@
       <c r="O150" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P150" s="3"/>
+      <c r="P150" s="65"/>
       <c r="Q150" s="3"/>
       <c r="R150" s="3"/>
       <c r="S150" s="3"/>
@@ -10736,6 +10872,7 @@
       <c r="O151" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P151" s="64"/>
     </row>
     <row r="152" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A152" s="4" t="s">
@@ -10783,7 +10920,7 @@
       <c r="O152" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P152" s="4"/>
+      <c r="P152" s="66"/>
       <c r="Q152" s="4"/>
       <c r="R152" s="4"/>
       <c r="S152" s="4"/>
@@ -10847,6 +10984,7 @@
       <c r="O153" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="P153" s="64"/>
     </row>
     <row r="154" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A154" s="19" t="s">
@@ -10892,7 +11030,7 @@
       <c r="O154" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P154" s="19"/>
+      <c r="P154" s="64"/>
       <c r="Q154" s="19"/>
       <c r="R154" s="19"/>
       <c r="S154" s="19"/>
@@ -10913,6 +11051,9 @@
       <c r="AH154" s="19"/>
       <c r="AI154" s="19"/>
     </row>
+    <row r="155" spans="1:35" x14ac:dyDescent="0.5">
+      <c r="P155" s="53"/>
+    </row>
     <row r="156" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A156" s="19" t="s">
         <v>320</v>
@@ -10930,25 +11071,29 @@
     <sortCondition ref="F2:F156"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC146917/"/>
-    <hyperlink ref="P3" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC146917/"/>
-    <hyperlink ref="P4" r:id="rId3" tooltip="Full text at publisher's site" display="http://onlinelibrary.wiley.com/resolve/openurl?genre=article&amp;sid=nlm:pubmed&amp;issn=0962-1083&amp;date=2003&amp;volume=12&amp;issue=5&amp;spage=1247"/>
-    <hyperlink ref="P5" r:id="rId4" tooltip="Full text at publisher's site" display="http://onlinelibrary.wiley.com/resolve/openurl?genre=article&amp;sid=nlm:pubmed&amp;issn=0962-1083&amp;date=2003&amp;volume=12&amp;issue=5&amp;spage=1247"/>
-    <hyperlink ref="P7" r:id="rId5" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1276035/"/>
-    <hyperlink ref="P8" r:id="rId6" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1276035/"/>
-    <hyperlink ref="P11" r:id="rId7" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25217773&amp;dopt=Abstract"/>
-    <hyperlink ref="P12" r:id="rId8" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25664748&amp;dopt=Abstract"/>
-    <hyperlink ref="P13" r:id="rId9" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19161942&amp;dopt=Abstract"/>
-    <hyperlink ref="P14" r:id="rId10" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16895613&amp;dopt=Abstract"/>
+    <hyperlink ref="P2" r:id="rId1" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=10872231&amp;dopt=Abstract"/>
+    <hyperlink ref="P3" r:id="rId2" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16258017&amp;dopt=Abstract"/>
+    <hyperlink ref="P7" r:id="rId3" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16081412&amp;dopt=Abstract"/>
+    <hyperlink ref="P8" r:id="rId4" display="http://link.springer.com/article/10.1007%2FBF00049339"/>
+    <hyperlink ref="P9" r:id="rId5" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12226484&amp;dopt=Abstract"/>
+    <hyperlink ref="P10" r:id="rId6" display="http://www.sciencedirect.com/science/article/pii/S0378111902011770"/>
+    <hyperlink ref="P12" r:id="rId7" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26734024&amp;dopt=Abstract"/>
+    <hyperlink ref="P13" r:id="rId8" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17015446&amp;dopt=Abstract"/>
+    <hyperlink ref="P15" r:id="rId9" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=15130548&amp;dopt=Abstract"/>
+    <hyperlink ref="P18" r:id="rId10" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16623885&amp;dopt=Abstract"/>
     <hyperlink ref="P19" r:id="rId11" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20650897&amp;dopt=Abstract"/>
-    <hyperlink ref="P20" r:id="rId12" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20650897&amp;dopt=Abstract"/>
-    <hyperlink ref="P6" r:id="rId13" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2528102/"/>
-    <hyperlink ref="P9" r:id="rId14" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1276035/"/>
-    <hyperlink ref="P10" r:id="rId15" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27855180&amp;dopt=Abstract"/>
-    <hyperlink ref="P15" r:id="rId16" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=15130548&amp;dopt=Abstract"/>
+    <hyperlink ref="P20" r:id="rId12" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20699392&amp;dopt=Abstract"/>
+    <hyperlink ref="P21" r:id="rId13" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC152217/"/>
+    <hyperlink ref="P22" r:id="rId14" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25966764&amp;dopt=Abstract"/>
+    <hyperlink ref="P24" r:id="rId15" display="https://www.ncbi.nlm.nih.gov/pubmed/16023399?dopt=Abstract"/>
+    <hyperlink ref="P25" r:id="rId16" display="https://www.ncbi.nlm.nih.gov/pubmed/8507825?dopt=Abstract"/>
+    <hyperlink ref="P26" r:id="rId17" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=15604686&amp;dopt=Abstract"/>
+    <hyperlink ref="P27" r:id="rId18" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17628825&amp;dopt=Abstract"/>
+    <hyperlink ref="P28" r:id="rId19" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=18365248&amp;dopt=Abstract"/>
+    <hyperlink ref="P29" r:id="rId20" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25669882&amp;dopt=Abstract"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId17"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added more reference files
</commit_message>
<xml_diff>
--- a/cold_genes_combined_with_gene_interval_update_01052017.xlsx
+++ b/cold_genes_combined_with_gene_interval_update_01052017.xlsx
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$157</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="461">
   <si>
     <t>Gene_Chr</t>
   </si>
@@ -1349,6 +1348,72 @@
   </si>
   <si>
     <t>OST1 Kinase Modulates Freezing Tolerance by Enhancing ICE1 Stability in Arabidopsis</t>
+  </si>
+  <si>
+    <t>Transcriptome analyses show changes in gene expression to accompany pollen germination and tube growth in Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Cellulose synthase complexes act in a concerted fashion to synthesize highly aggregated cellulose in secondary cell walls of plants</t>
+  </si>
+  <si>
+    <t>Regulation of plant immunity through ubiquitin-mediated modulation of Ca(2+) -calmodulin-AtSR1/CAMTA3 signaling</t>
+  </si>
+  <si>
+    <t>Expression of E. coli glycogen branching enzyme in an Arabidopsis mutant devoid of endogenous starch branching enzymes induces the synthesis of starch-like polyglucans</t>
+  </si>
+  <si>
+    <t>Starch metabolism in Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Point mutation of a plastidic invertase inhibits development of the photosynthetic apparatus and enhances nitrate assimilation in sugar-treated Arabidopsis seedlings</t>
+  </si>
+  <si>
+    <t>Exploring the neutral invertase-oxidative stress defence connection in Arabidopsis thaliana</t>
+  </si>
+  <si>
+    <t>Paired Hierarchical Organization of 13-Lipoxygenases in Arabidopsis</t>
+  </si>
+  <si>
+    <t>Arabidopsis lox3 lox4 double mutants are male sterile and defective in global proliferative arrest</t>
+  </si>
+  <si>
+    <t>Glycerol-3-Phosphate Acyltransferase 6 (GPAT6) Is Important for Tapetum Development in Arabidopsis and Plays Multiple Roles in Plant Fertility</t>
+  </si>
+  <si>
+    <t>Molecular Cloning and Expression of cor (Cold-Regulated) Genes in Arabidopsis thaliana</t>
+  </si>
+  <si>
+    <t>AtDGK2, a novel diacylglycerol kinase from Arabidopsis thaliana, phosphorylates 1-stearoyl-2-arachidonoyl-sn-glycerol and 1,2-dioleoyl-sn-glycerol, and exhibits cold-inducible gene expression.</t>
+  </si>
+  <si>
+    <t>Calcium Sensors and Their Interacting Protein Kinases: Genomics of the Arabidopsis and Rice CBL-CIPK Signaling Networks.</t>
+  </si>
+  <si>
+    <t>Plant protein inhibitors of invertases.</t>
+  </si>
+  <si>
+    <t>Soybean GmbZIP123 gene enhances lipid content in the seeds of transgenic Arabidopsis plants</t>
+  </si>
+  <si>
+    <t>Structural basis of the regulatory mechanism of the plant CIPK family of protein kinases controlling ion homeostasis and abiotic stress</t>
+  </si>
+  <si>
+    <t>Genome-wide and expression analysis of protein phosphatase 2C in rice and Arabidopsis.</t>
+  </si>
+  <si>
+    <t>DWARF TILLER1, a WUSCHEL-Related Homeobox Transcription Factor, Is Required for Tiller Growth in Rice</t>
+  </si>
+  <si>
+    <t>UDP-glucose pyrophosphorylase is rate limiting in vegetative and reproductive phases in Arabidopsis thaliana</t>
+  </si>
+  <si>
+    <t>Impairment of Cellulose Synthases Required for Arabidopsis Secondary Cell Wall Formation Enhances Disease Resistance.</t>
+  </si>
+  <si>
+    <t>Four Arabidopsis?AREB/ABF transcription factors function predominantly in gene expression downstream of SnRK2 kinases in abscisic acid signalling in response to osmotic stress</t>
+  </si>
+  <si>
+    <t>The Role of Cytosolic alpha-Glucan Phosphorylase in Maltose Metabolism and the Comparison of Amylomaltase in Arabidopsis and E. coli.</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1857,6 +1922,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2164,8 +2232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="N22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q59" sqref="Q59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.4" x14ac:dyDescent="0.5"/>
@@ -3841,7 +3909,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="4" t="s">
         <v>300</v>
       </c>
@@ -3887,8 +3955,12 @@
       <c r="O30" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P30" s="66"/>
-      <c r="Q30" s="4"/>
+      <c r="P30" s="55">
+        <v>18775970</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>439</v>
+      </c>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
@@ -3908,7 +3980,7 @@
       <c r="AH30" s="4"/>
       <c r="AI30" s="4"/>
     </row>
-    <row r="31" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="19" t="s">
         <v>255</v>
       </c>
@@ -3952,8 +4024,12 @@
       <c r="O31" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P31" s="64"/>
-      <c r="Q31" s="19"/>
+      <c r="P31" s="57">
+        <v>27647923</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>440</v>
+      </c>
       <c r="R31" s="19"/>
       <c r="S31" s="19"/>
       <c r="T31" s="19"/>
@@ -3973,7 +4049,7 @@
       <c r="AH31" s="19"/>
       <c r="AI31" s="19"/>
     </row>
-    <row r="32" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A32" s="19" t="s">
         <v>258</v>
       </c>
@@ -4017,8 +4093,12 @@
       <c r="O32" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="19"/>
+      <c r="P32" s="55">
+        <v>24528504</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>441</v>
+      </c>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
       <c r="T32" s="19"/>
@@ -4038,7 +4118,7 @@
       <c r="AH32" s="19"/>
       <c r="AI32" s="19"/>
     </row>
-    <row r="33" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A33" s="19" t="s">
         <v>293</v>
       </c>
@@ -4082,8 +4162,12 @@
       <c r="O33" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P33" s="64"/>
-      <c r="Q33" s="19"/>
+      <c r="P33" s="55">
+        <v>26715025</v>
+      </c>
+      <c r="Q33" s="19" t="s">
+        <v>442</v>
+      </c>
       <c r="R33" s="19"/>
       <c r="S33" s="19"/>
       <c r="T33" s="19"/>
@@ -4147,8 +4231,12 @@
       <c r="O34" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P34" s="66"/>
-      <c r="Q34" s="4"/>
+      <c r="P34" s="55">
+        <v>23393426</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>443</v>
+      </c>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
@@ -4168,7 +4256,7 @@
       <c r="AH34" s="4"/>
       <c r="AI34" s="4"/>
     </row>
-    <row r="35" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
         <v>280</v>
       </c>
@@ -4214,9 +4302,14 @@
       <c r="O35" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P35" s="65"/>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.5">
+      <c r="P35" s="57">
+        <v>20304912</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A36" s="21" t="s">
         <v>280</v>
       </c>
@@ -4259,7 +4352,12 @@
       <c r="O36" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P36" s="53"/>
+      <c r="P36" s="55">
+        <v>21441406</v>
+      </c>
+      <c r="Q36" s="21" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="37" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A37" s="28" t="s">
@@ -4307,8 +4405,12 @@
       <c r="O37" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="21"/>
+      <c r="P37" s="57">
+        <v>21052784</v>
+      </c>
+      <c r="Q37" s="21" t="s">
+        <v>447</v>
+      </c>
       <c r="R37" s="21"/>
       <c r="S37" s="21"/>
       <c r="T37" s="21"/>
@@ -4371,7 +4473,12 @@
       <c r="O38" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P38" s="64"/>
+      <c r="P38" s="55">
+        <v>21746699</v>
+      </c>
+      <c r="Q38" s="19" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A39" s="19" t="s">
@@ -4482,8 +4589,12 @@
       <c r="O40" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="19"/>
+      <c r="P40" s="73">
+        <v>1062659</v>
+      </c>
+      <c r="Q40" s="19" t="s">
+        <v>449</v>
+      </c>
       <c r="R40" s="19"/>
       <c r="S40" s="19"/>
       <c r="T40" s="19"/>
@@ -4757,7 +4868,7 @@
       <c r="AH44" s="21"/>
       <c r="AI44" s="21"/>
     </row>
-    <row r="45" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A45" s="19" t="s">
         <v>17</v>
       </c>
@@ -4800,9 +4911,14 @@
       <c r="O45" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P45" s="64"/>
-    </row>
-    <row r="46" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="P45" s="55">
+        <v>14665624</v>
+      </c>
+      <c r="Q45" s="19" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A46" s="19" t="s">
         <v>226</v>
       </c>
@@ -4845,9 +4961,14 @@
       <c r="O46" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P46" s="64"/>
-    </row>
-    <row r="47" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="P46" s="55">
+        <v>14730064</v>
+      </c>
+      <c r="Q46" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A47" s="19" t="s">
         <v>280</v>
       </c>
@@ -4890,9 +5011,14 @@
       <c r="O47" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P47" s="64"/>
-    </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.5">
+      <c r="P47" s="55">
+        <v>14871666</v>
+      </c>
+      <c r="Q47" s="19" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A48" s="19" t="s">
         <v>280</v>
       </c>
@@ -4936,8 +5062,12 @@
       <c r="O48" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P48" s="64"/>
-      <c r="Q48" s="19"/>
+      <c r="P48" s="55">
+        <v>23963672</v>
+      </c>
+      <c r="Q48" s="19" t="s">
+        <v>453</v>
+      </c>
       <c r="R48" s="19"/>
       <c r="S48" s="19"/>
       <c r="T48" s="19"/>
@@ -5066,8 +5196,12 @@
       <c r="O50" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P50" s="64"/>
-      <c r="Q50" s="19"/>
+      <c r="P50" s="55">
+        <v>25288725</v>
+      </c>
+      <c r="Q50" s="19" t="s">
+        <v>454</v>
+      </c>
       <c r="R50" s="19"/>
       <c r="S50" s="19"/>
       <c r="T50" s="19"/>
@@ -5259,8 +5393,12 @@
       <c r="O53" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P53" s="66"/>
-      <c r="Q53" s="4"/>
+      <c r="P53" s="55">
+        <v>19021904</v>
+      </c>
+      <c r="Q53" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
       <c r="T53" s="4"/>
@@ -5326,8 +5464,12 @@
       <c r="O54" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="P54" s="67"/>
-      <c r="Q54" s="36"/>
+      <c r="P54" s="55">
+        <v>24625559</v>
+      </c>
+      <c r="Q54" s="36" t="s">
+        <v>456</v>
+      </c>
       <c r="R54" s="36"/>
       <c r="S54" s="36"/>
       <c r="T54" s="36"/>
@@ -5391,8 +5533,12 @@
       <c r="O55" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="21"/>
+      <c r="P55" s="55">
+        <v>20435647</v>
+      </c>
+      <c r="Q55" s="21" t="s">
+        <v>457</v>
+      </c>
       <c r="R55" s="21"/>
       <c r="S55" s="21"/>
       <c r="T55" s="21"/>
@@ -5412,7 +5558,7 @@
       <c r="AH55" s="21"/>
       <c r="AI55" s="21"/>
     </row>
-    <row r="56" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A56" s="4" t="s">
         <v>255</v>
       </c>
@@ -5458,8 +5604,12 @@
       <c r="O56" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P56" s="66"/>
-      <c r="Q56" s="4"/>
+      <c r="P56" s="55">
+        <v>17351116</v>
+      </c>
+      <c r="Q56" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="R56" s="4"/>
       <c r="S56" s="4"/>
       <c r="T56" s="4"/>
@@ -5525,8 +5675,12 @@
       <c r="O57" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P57" s="65"/>
-      <c r="Q57" s="3"/>
+      <c r="P57" s="57">
+        <v>24738645</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>459</v>
+      </c>
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
@@ -5648,7 +5802,12 @@
       <c r="O59" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P59" s="53"/>
+      <c r="P59" s="55">
+        <v>16980562</v>
+      </c>
+      <c r="Q59" s="21" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="60" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A60" s="19" t="s">
@@ -6940,7 +7099,7 @@
       <c r="AH82" s="3"/>
       <c r="AI82" s="3"/>
     </row>
-    <row r="83" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A83" s="4" t="s">
         <v>297</v>
       </c>
@@ -6986,7 +7145,12 @@
       <c r="O83" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P83" s="66"/>
+      <c r="P83" s="57">
+        <v>27135236</v>
+      </c>
+      <c r="Q83" s="4" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="84" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="s">
@@ -11091,9 +11255,31 @@
     <hyperlink ref="P27" r:id="rId18" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17628825&amp;dopt=Abstract"/>
     <hyperlink ref="P28" r:id="rId19" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=18365248&amp;dopt=Abstract"/>
     <hyperlink ref="P29" r:id="rId20" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25669882&amp;dopt=Abstract"/>
+    <hyperlink ref="P30" r:id="rId21" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=18775970&amp;dopt=Abstract"/>
+    <hyperlink ref="P31" r:id="rId22" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27647923&amp;dopt=Abstract"/>
+    <hyperlink ref="P32" r:id="rId23" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24528504&amp;dopt=Abstract"/>
+    <hyperlink ref="P33" r:id="rId24" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26715025&amp;dopt=Abstract"/>
+    <hyperlink ref="P34" r:id="rId25" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23393426&amp;dopt=Abstract"/>
+    <hyperlink ref="P35" r:id="rId26" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20304912&amp;dopt=Abstract"/>
+    <hyperlink ref="P36" r:id="rId27" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21441406&amp;dopt=Abstract"/>
+    <hyperlink ref="P83" r:id="rId28" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27135236&amp;dopt=Abstract"/>
+    <hyperlink ref="P37" r:id="rId29" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21052784&amp;dopt=Abstract"/>
+    <hyperlink ref="P38" r:id="rId30" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21746699&amp;dopt=Abstract"/>
+    <hyperlink ref="P40" r:id="rId31" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1062659/"/>
+    <hyperlink ref="P45" r:id="rId32" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14665624&amp;dopt=Abstract"/>
+    <hyperlink ref="P46" r:id="rId33" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14730064&amp;dopt=Abstract"/>
+    <hyperlink ref="P47" r:id="rId34" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14871666&amp;dopt=Abstract"/>
+    <hyperlink ref="P48" r:id="rId35" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23963672&amp;dopt=Abstract"/>
+    <hyperlink ref="P50" r:id="rId36" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25288725&amp;dopt=Abstract"/>
+    <hyperlink ref="P53" r:id="rId37" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19021904&amp;dopt=Abstract"/>
+    <hyperlink ref="P54" r:id="rId38" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24625559&amp;dopt=Abstract"/>
+    <hyperlink ref="P55" r:id="rId39" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20435647&amp;dopt=Abstract"/>
+    <hyperlink ref="P56" r:id="rId40" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17351116&amp;dopt=Abstract"/>
+    <hyperlink ref="P57" r:id="rId41" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24738645&amp;dopt=Abstract"/>
+    <hyperlink ref="P59" r:id="rId42" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16980562&amp;dopt=Abstract"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId21"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId43"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
looked up Oryza sativa with NCBI. Didn't find much
</commit_message>
<xml_diff>
--- a/cold_genes_combined_with_gene_interval_update_01052017.xlsx
+++ b/cold_genes_combined_with_gene_interval_update_01052017.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="502">
   <si>
     <t>Gene_Chr</t>
   </si>
@@ -1522,13 +1522,28 @@
   </si>
   <si>
     <t>REVEILLE1, a Myb-like transcription factor, integrates the circadian clock and auxin pathways</t>
+  </si>
+  <si>
+    <t>Collection, mapping, and annotation of over 28,000 cDNA clones from japonica rice.</t>
+  </si>
+  <si>
+    <t>Inducible overexpression of a rice allene oxide synthase gene increases the endogenous jasmonic acid level, PR gene expression, and host resistance to fungal infection.</t>
+  </si>
+  <si>
+    <t>Sequence and analysis of rice chromosome 4.</t>
+  </si>
+  <si>
+    <t>Functional Analysis of an Arabidopsis Transcription Factor, DREB2A, Involved in Drought-Responsive Gene Expression</t>
+  </si>
+  <si>
+    <t>A network of rice genes associated with stress response and seed development.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1682,6 +1697,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="4"/>
+      <color rgb="FF575757"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1819,7 +1840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2028,6 +2049,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2334,7 +2356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
@@ -2577,8 +2599,12 @@
       <c r="O4" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="61"/>
+      <c r="P4" s="55">
+        <v>12869764</v>
+      </c>
+      <c r="Q4" s="68" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="5" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="17" t="s">
@@ -6951,8 +6977,12 @@
       <c r="O77" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P77" s="64"/>
-      <c r="Q77" s="19"/>
+      <c r="P77" s="69">
+        <v>17022177</v>
+      </c>
+      <c r="Q77" s="19" t="s">
+        <v>498</v>
+      </c>
       <c r="R77" s="19"/>
       <c r="S77" s="19"/>
       <c r="T77" s="19"/>
@@ -6972,7 +7002,7 @@
       <c r="AH77" s="19"/>
       <c r="AI77" s="19"/>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A78" s="19" t="s">
         <v>371</v>
       </c>
@@ -7016,7 +7046,7 @@
       <c r="O78" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P78" s="64"/>
+      <c r="P78" s="72"/>
       <c r="Q78" s="19"/>
       <c r="R78" s="19"/>
       <c r="S78" s="19"/>
@@ -8250,7 +8280,7 @@
       </c>
       <c r="P98" s="53"/>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A99" s="21" t="s">
         <v>267</v>
       </c>
@@ -8293,9 +8323,14 @@
       <c r="O99" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P99" s="53"/>
-    </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.5">
+      <c r="P99" s="69">
+        <v>12447439</v>
+      </c>
+      <c r="Q99" s="21" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="100" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A100" s="21" t="s">
         <v>267</v>
       </c>
@@ -8338,7 +8373,7 @@
       <c r="O100" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P100" s="53"/>
+      <c r="P100" s="72"/>
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A101" s="21" t="s">
@@ -8495,7 +8530,7 @@
       <c r="AH103" s="19"/>
       <c r="AI103" s="19"/>
     </row>
-    <row r="104" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A104" s="21" t="s">
         <v>265</v>
       </c>
@@ -8539,8 +8574,12 @@
       <c r="O104" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P104" s="53"/>
-      <c r="Q104" s="21"/>
+      <c r="P104" s="55">
+        <v>1456870</v>
+      </c>
+      <c r="Q104" s="21" t="s">
+        <v>500</v>
+      </c>
       <c r="R104" s="21"/>
       <c r="S104" s="21"/>
       <c r="T104" s="21"/>
@@ -11321,7 +11360,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="152" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A152" s="4" t="s">
         <v>178</v>
       </c>
@@ -11367,8 +11406,12 @@
       <c r="O152" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P152" s="66"/>
-      <c r="Q152" s="4"/>
+      <c r="P152" s="55">
+        <v>153660</v>
+      </c>
+      <c r="Q152" s="4" t="s">
+        <v>501</v>
+      </c>
       <c r="R152" s="4"/>
       <c r="S152" s="4"/>
       <c r="T152" s="4"/>
@@ -11606,9 +11649,14 @@
     <hyperlink ref="P145" r:id="rId81" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12383501&amp;dopt=Abstract"/>
     <hyperlink ref="P151" r:id="rId82" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17587236&amp;dopt=Abstract"/>
     <hyperlink ref="P150" r:id="rId83" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19805390&amp;dopt=Abstract"/>
+    <hyperlink ref="P4" r:id="rId84" display="https://www.ncbi.nlm.nih.gov/pubmed/12869764"/>
+    <hyperlink ref="P77" r:id="rId85" display="https://www.ncbi.nlm.nih.gov/pubmed/17022177"/>
+    <hyperlink ref="P99" r:id="rId86" display="https://www.ncbi.nlm.nih.gov/pubmed/12447439"/>
+    <hyperlink ref="P104" r:id="rId87" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1456870/"/>
+    <hyperlink ref="P152" r:id="rId88" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC153660/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId84"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId89"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
looked up Hordeum with NCBI. Didn't find much
</commit_message>
<xml_diff>
--- a/cold_genes_combined_with_gene_interval_update_01052017.xlsx
+++ b/cold_genes_combined_with_gene_interval_update_01052017.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="509">
   <si>
     <t>Gene_Chr</t>
   </si>
@@ -1537,13 +1537,34 @@
   </si>
   <si>
     <t>A network of rice genes associated with stress response and seed development.</t>
+  </si>
+  <si>
+    <t>Mapping of barley homologs to genes that regulate low temperature tolerance in Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Structural, functional, and phylogenetic characterization of a large CBF gene family in barley.</t>
+  </si>
+  <si>
+    <t>CBF gene copy number variation at Frost Resistance-2 is associated with levels of freezing tolerance in temperate-climate cereals.</t>
+  </si>
+  <si>
+    <t>Barley Cbf3 gene identification, expression pattern, and map location.</t>
+  </si>
+  <si>
+    <t>Mapping-by-sequencing accelerates forward genetics in barley.</t>
+  </si>
+  <si>
+    <t>Characterization of a calmodulin-binding transporter from the plasma membrane of barley aleurone.</t>
+  </si>
+  <si>
+    <t>Transcriptome analysis of high-temperature stress in developing barley caryopses: early stress responses and effects on storage compound biosynthesis.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1703,6 +1724,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF575757"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1840,7 +1867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2050,6 +2077,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6108,7 +6136,7 @@
       <c r="AH62" s="4"/>
       <c r="AI62" s="4"/>
     </row>
-    <row r="63" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A63" s="4" t="s">
         <v>247</v>
       </c>
@@ -6154,8 +6182,12 @@
       <c r="O63" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P63" s="66"/>
-      <c r="Q63" s="4"/>
+      <c r="P63" s="55">
+        <v>16365758</v>
+      </c>
+      <c r="Q63" s="4" t="s">
+        <v>502</v>
+      </c>
       <c r="R63" s="4"/>
       <c r="S63" s="4"/>
       <c r="T63" s="4"/>
@@ -7228,7 +7260,7 @@
       <c r="AH81" s="21"/>
       <c r="AI81" s="21"/>
     </row>
-    <row r="82" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A82" s="3" t="s">
         <v>198</v>
       </c>
@@ -7274,8 +7306,12 @@
       <c r="O82" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P82" s="65"/>
-      <c r="Q82" s="3"/>
+      <c r="P82" s="55">
+        <v>12559580</v>
+      </c>
+      <c r="Q82" s="3" t="s">
+        <v>423</v>
+      </c>
       <c r="R82" s="3"/>
       <c r="S82" s="3"/>
       <c r="T82" s="3"/>
@@ -8170,7 +8206,7 @@
       <c r="AH96" s="19"/>
       <c r="AI96" s="19"/>
     </row>
-    <row r="97" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:35" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A97" s="21" t="s">
         <v>252</v>
       </c>
@@ -8214,8 +8250,12 @@
       <c r="O97" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P97" s="53"/>
-      <c r="Q97" s="21"/>
+      <c r="P97" s="55">
+        <v>16244905</v>
+      </c>
+      <c r="Q97" s="21" t="s">
+        <v>503</v>
+      </c>
       <c r="R97" s="21"/>
       <c r="S97" s="21"/>
       <c r="T97" s="21"/>
@@ -8235,7 +8275,7 @@
       <c r="AH97" s="21"/>
       <c r="AI97" s="21"/>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A98" s="21" t="s">
         <v>252</v>
       </c>
@@ -8278,7 +8318,12 @@
       <c r="O98" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P98" s="53"/>
+      <c r="P98" s="55">
+        <v>16365758</v>
+      </c>
+      <c r="Q98" s="21" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="99" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A99" s="21" t="s">
@@ -8330,7 +8375,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:35" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A100" s="21" t="s">
         <v>267</v>
       </c>
@@ -8373,7 +8418,12 @@
       <c r="O100" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P100" s="72"/>
+      <c r="P100" s="55">
+        <v>20213518</v>
+      </c>
+      <c r="Q100" s="21" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.5">
       <c r="A101" s="21" t="s">
@@ -8599,7 +8649,7 @@
       <c r="AH104" s="21"/>
       <c r="AI104" s="21"/>
     </row>
-    <row r="105" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A105" s="21" t="s">
         <v>265</v>
       </c>
@@ -8643,8 +8693,12 @@
       <c r="O105" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P105" s="53"/>
-      <c r="Q105" s="21"/>
+      <c r="P105" s="69">
+        <v>12177491</v>
+      </c>
+      <c r="Q105" s="21" t="s">
+        <v>505</v>
+      </c>
       <c r="R105" s="21"/>
       <c r="S105" s="21"/>
       <c r="T105" s="21"/>
@@ -8664,7 +8718,7 @@
       <c r="AH105" s="21"/>
       <c r="AI105" s="21"/>
     </row>
-    <row r="106" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="21" t="s">
         <v>291</v>
       </c>
@@ -8708,7 +8762,7 @@
       <c r="O106" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P106" s="53"/>
+      <c r="P106" s="73"/>
       <c r="Q106" s="21"/>
       <c r="R106" s="21"/>
       <c r="S106" s="21"/>
@@ -9100,7 +9154,12 @@
       <c r="O112" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P112" s="64"/>
+      <c r="P112" s="55">
+        <v>24917130</v>
+      </c>
+      <c r="Q112" s="19" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="113" spans="1:35" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A113" s="19" t="s">
@@ -11062,7 +11121,12 @@
       <c r="O146" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P146" s="64"/>
+      <c r="P146" s="55">
+        <v>9465122</v>
+      </c>
+      <c r="Q146" s="19" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="147" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A147" s="19" t="s">
@@ -11151,8 +11215,12 @@
       <c r="O148" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P148" s="53"/>
-      <c r="Q148" s="21"/>
+      <c r="P148" s="69">
+        <v>20924027</v>
+      </c>
+      <c r="Q148" s="21" t="s">
+        <v>508</v>
+      </c>
       <c r="R148" s="21"/>
       <c r="S148" s="21"/>
       <c r="T148" s="21"/>
@@ -11172,7 +11240,7 @@
       <c r="AH148" s="21"/>
       <c r="AI148" s="21"/>
     </row>
-    <row r="149" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:35" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A149" s="3" t="s">
         <v>76</v>
       </c>
@@ -11218,7 +11286,7 @@
       <c r="O149" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P149" s="65"/>
+      <c r="P149" s="72"/>
       <c r="Q149" s="3"/>
       <c r="R149" s="3"/>
       <c r="S149" s="3"/>
@@ -11654,9 +11722,18 @@
     <hyperlink ref="P99" r:id="rId86" display="https://www.ncbi.nlm.nih.gov/pubmed/12447439"/>
     <hyperlink ref="P104" r:id="rId87" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1456870/"/>
     <hyperlink ref="P152" r:id="rId88" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC153660/"/>
+    <hyperlink ref="P63" r:id="rId89" display="https://www.ncbi.nlm.nih.gov/pubmed/16365758"/>
+    <hyperlink ref="P82" r:id="rId90" display="https://www.ncbi.nlm.nih.gov/pubmed/12559580"/>
+    <hyperlink ref="P97" r:id="rId91" display="https://www.ncbi.nlm.nih.gov/pubmed/16244905"/>
+    <hyperlink ref="P98" r:id="rId92" display="https://www.ncbi.nlm.nih.gov/pubmed/16365758"/>
+    <hyperlink ref="P100" r:id="rId93" display="https://www.ncbi.nlm.nih.gov/pubmed/20213518"/>
+    <hyperlink ref="P105" r:id="rId94" display="https://www.ncbi.nlm.nih.gov/pubmed/12177491"/>
+    <hyperlink ref="P112" r:id="rId95" display="https://www.ncbi.nlm.nih.gov/pubmed/24917130"/>
+    <hyperlink ref="P146" r:id="rId96" display="https://www.ncbi.nlm.nih.gov/pubmed/9465122"/>
+    <hyperlink ref="P148" r:id="rId97" display="https://www.ncbi.nlm.nih.gov/pubmed/20924027"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId89"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId98"/>
 </worksheet>
 </file>
 

</xml_diff>